<commit_message>
remove useless fields of template
</commit_message>
<xml_diff>
--- a/Quality2/wwwroot/template.xlsx
+++ b/Quality2/wwwroot/template.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>ОБЩЕСТВО С ОГРАНИЧЕННОЙ ОТВЕТСТВЕННОСТЬЮ</t>
   </si>
@@ -39,22 +39,10 @@
     <t>ПАСПОРТ</t>
   </si>
   <si>
-    <t>Толщина</t>
-  </si>
-  <si>
-    <t>Ширина</t>
-  </si>
-  <si>
-    <t>Цвет</t>
-  </si>
-  <si>
     <t>Наименование продукта</t>
   </si>
   <si>
     <t>"ПЛЕНКА ПОЛИМЕРНАЯ, МНОГОСЛОЙНАЯ</t>
-  </si>
-  <si>
-    <t>белый</t>
   </si>
   <si>
     <t>ТУ 22.21.30-002-03210778-2022</t>
@@ -775,219 +763,19 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1026,6 +814,206 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -20677,19 +20665,19 @@
       <c r="P3" s="4"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A4" s="81" t="s">
+      <c r="A4" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="82"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="27"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
@@ -20697,19 +20685,19 @@
       <c r="P4" s="4"/>
     </row>
     <row r="5" spans="1:16" ht="30" x14ac:dyDescent="0.45">
-      <c r="A5" s="83" t="s">
+      <c r="A5" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="84"/>
-      <c r="C5" s="84"/>
-      <c r="D5" s="84"/>
-      <c r="E5" s="84"/>
-      <c r="F5" s="84"/>
-      <c r="G5" s="84"/>
-      <c r="H5" s="84"/>
-      <c r="I5" s="84"/>
-      <c r="J5" s="84"/>
-      <c r="K5" s="85"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="30"/>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
@@ -20717,19 +20705,19 @@
       <c r="P5" s="4"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A6" s="86" t="s">
+      <c r="A6" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="87"/>
-      <c r="C6" s="87"/>
-      <c r="D6" s="87"/>
-      <c r="E6" s="87"/>
-      <c r="F6" s="87"/>
-      <c r="G6" s="87"/>
-      <c r="H6" s="87"/>
-      <c r="I6" s="87"/>
-      <c r="J6" s="87"/>
-      <c r="K6" s="88"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="32"/>
+      <c r="K6" s="33"/>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
@@ -20758,17 +20746,17 @@
       <c r="A8" s="5"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
-      <c r="D8" s="89" t="s">
+      <c r="D8" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="89"/>
-      <c r="F8" s="89"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="8">
         <f>E14</f>
         <v>1349</v>
       </c>
-      <c r="H8" s="90"/>
-      <c r="I8" s="24"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="26"/>
       <c r="J8" s="6"/>
       <c r="K8" s="7"/>
       <c r="L8" s="4"/>
@@ -20790,90 +20778,70 @@
       <c r="J9" s="6"/>
       <c r="K9" s="7"/>
       <c r="L9" s="4"/>
-      <c r="M9" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="N9" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="O9" s="9" t="s">
-        <v>6</v>
-      </c>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
       <c r="P9" s="9"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A10" s="10"/>
-      <c r="B10" s="67" t="s">
-        <v>7</v>
+      <c r="B10" s="23" t="s">
+        <v>4</v>
       </c>
-      <c r="C10" s="67"/>
-      <c r="D10" s="67"/>
-      <c r="E10" s="74" t="s">
-        <v>8</v>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="24" t="s">
+        <v>5</v>
       </c>
-      <c r="F10" s="74"/>
-      <c r="G10" s="74"/>
-      <c r="H10" s="74"/>
-      <c r="I10" s="74"/>
-      <c r="J10" s="74"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
       <c r="K10" s="7"/>
       <c r="L10" s="4"/>
-      <c r="M10" s="11">
-        <f>VLOOKUP($E$14,[1]Данные!$A2:$W500,10,FALSE)/1000</f>
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="N10" s="9">
-        <f>VLOOKUP($E$14,[1]Данные!$A2:$W500,9,FALSE)</f>
-        <v>615</v>
-      </c>
-      <c r="O10" s="9" t="str">
-        <f>VLOOKUP($E$14,[1]Данные!$A2:$W500,8,FALSE)</f>
-        <v>прозрачный</v>
-      </c>
+      <c r="M10" s="11"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
       <c r="P10" s="9"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A11" s="5"/>
       <c r="B11" s="6"/>
-      <c r="C11" s="76" t="str">
+      <c r="C11" s="36" t="str">
         <f>CONCATENATE(N10,"Х",M10," мм",","," ","марка")</f>
-        <v>615Х0,025 мм, марка</v>
+        <v>Х мм, марка</v>
       </c>
-      <c r="D11" s="76"/>
-      <c r="E11" s="76"/>
-      <c r="F11" s="76"/>
-      <c r="G11" s="76"/>
-      <c r="H11" s="77" t="str">
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="37" t="str">
         <f>VLOOKUP($E$14,[1]Данные!$A2:$W500,7,FALSE)</f>
         <v>Л</v>
       </c>
-      <c r="I11" s="77"/>
-      <c r="J11" s="77"/>
+      <c r="I11" s="37"/>
+      <c r="J11" s="37"/>
       <c r="K11" s="7"/>
       <c r="L11" s="4"/>
-      <c r="M11" s="9">
-        <f>VLOOKUP($E$14,[1]Данные!$A2:$W500,10,FALSE)</f>
-        <v>25</v>
-      </c>
+      <c r="M11" s="9"/>
       <c r="N11" s="9"/>
       <c r="O11" s="9"/>
-      <c r="P11" s="9" t="s">
-        <v>9</v>
-      </c>
+      <c r="P11" s="9"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="78" t="s">
-        <v>10</v>
+      <c r="C12" s="38" t="s">
+        <v>6</v>
       </c>
-      <c r="D12" s="78"/>
-      <c r="E12" s="78"/>
-      <c r="F12" s="78"/>
-      <c r="G12" s="78"/>
-      <c r="H12" s="78"/>
-      <c r="I12" s="78"/>
-      <c r="J12" s="78"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
       <c r="K12" s="7"/>
       <c r="L12" s="4"/>
       <c r="M12" s="9"/>
@@ -20883,15 +20851,15 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A13" s="5"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="23"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="39"/>
+      <c r="J13" s="39"/>
       <c r="K13" s="7"/>
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
@@ -20901,23 +20869,23 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A14" s="5"/>
-      <c r="B14" s="24" t="s">
-        <v>11</v>
+      <c r="B14" s="26" t="s">
+        <v>7</v>
       </c>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="79">
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="40">
         <v>1349</v>
       </c>
-      <c r="F14" s="79"/>
+      <c r="F14" s="40"/>
       <c r="G14" s="12" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
-      <c r="H14" s="80" t="str">
+      <c r="H14" s="41" t="str">
         <f>TEXT(VLOOKUP($E$14,[1]Данные!$A2:$W500,8,FALSE),1)</f>
         <v>прозрачный</v>
       </c>
-      <c r="I14" s="80"/>
+      <c r="I14" s="41"/>
       <c r="J14" s="6"/>
       <c r="K14" s="7"/>
       <c r="L14" s="4"/>
@@ -20928,14 +20896,14 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A15" s="5"/>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="23"/>
+      <c r="B15" s="39"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="39"/>
+      <c r="I15" s="39"/>
       <c r="J15" s="6"/>
       <c r="K15" s="7"/>
       <c r="L15" s="4"/>
@@ -20946,16 +20914,16 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A16" s="5"/>
-      <c r="B16" s="67" t="s">
-        <v>13</v>
+      <c r="B16" s="23" t="s">
+        <v>9</v>
       </c>
-      <c r="C16" s="67"/>
-      <c r="D16" s="67"/>
-      <c r="E16" s="67"/>
-      <c r="F16" s="67"/>
-      <c r="G16" s="74"/>
-      <c r="H16" s="74"/>
-      <c r="I16" s="74"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
       <c r="J16" s="6"/>
       <c r="K16" s="7"/>
       <c r="L16" s="4"/>
@@ -20966,14 +20934,14 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A17" s="5"/>
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="23"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="39"/>
+      <c r="I17" s="39"/>
       <c r="J17" s="6"/>
       <c r="K17" s="7"/>
       <c r="L17" s="4"/>
@@ -20984,16 +20952,16 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A18" s="5"/>
-      <c r="B18" s="67" t="s">
-        <v>14</v>
+      <c r="B18" s="23" t="s">
+        <v>10</v>
       </c>
-      <c r="C18" s="67"/>
-      <c r="D18" s="67"/>
-      <c r="E18" s="75"/>
-      <c r="F18" s="75"/>
-      <c r="G18" s="75"/>
-      <c r="H18" s="75"/>
-      <c r="I18" s="75"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
       <c r="J18" s="6"/>
       <c r="K18" s="7"/>
       <c r="L18" s="4"/>
@@ -21004,14 +20972,14 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A19" s="5"/>
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="23"/>
-      <c r="I19" s="23"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="39"/>
+      <c r="I19" s="39"/>
       <c r="J19" s="6"/>
       <c r="K19" s="7"/>
       <c r="L19" s="4"/>
@@ -21022,18 +20990,18 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A20" s="5"/>
-      <c r="B20" s="67" t="s">
-        <v>15</v>
+      <c r="B20" s="23" t="s">
+        <v>11</v>
       </c>
-      <c r="C20" s="67"/>
-      <c r="D20" s="67"/>
-      <c r="E20" s="68" t="s">
-        <v>39</v>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="43" t="s">
+        <v>35</v>
       </c>
-      <c r="F20" s="69"/>
-      <c r="G20" s="69"/>
-      <c r="H20" s="69"/>
-      <c r="I20" s="69"/>
+      <c r="F20" s="44"/>
+      <c r="G20" s="44"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="44"/>
       <c r="J20" s="6"/>
       <c r="K20" s="7"/>
       <c r="L20" s="4"/>
@@ -21044,14 +21012,14 @@
     </row>
     <row r="21" spans="1:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A21" s="5"/>
-      <c r="B21" s="70"/>
-      <c r="C21" s="70"/>
-      <c r="D21" s="70"/>
-      <c r="E21" s="70"/>
-      <c r="F21" s="70"/>
-      <c r="G21" s="70"/>
-      <c r="H21" s="70"/>
-      <c r="I21" s="70"/>
+      <c r="B21" s="45"/>
+      <c r="C21" s="45"/>
+      <c r="D21" s="45"/>
+      <c r="E21" s="45"/>
+      <c r="F21" s="45"/>
+      <c r="G21" s="45"/>
+      <c r="H21" s="45"/>
+      <c r="I21" s="45"/>
       <c r="J21" s="6"/>
       <c r="K21" s="7"/>
       <c r="L21" s="4"/>
@@ -21063,22 +21031,22 @@
     <row r="22" spans="1:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A22" s="5"/>
       <c r="B22" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
-      <c r="C22" s="71" t="s">
-        <v>17</v>
+      <c r="C22" s="46" t="s">
+        <v>13</v>
       </c>
-      <c r="D22" s="72"/>
-      <c r="E22" s="73"/>
-      <c r="F22" s="71" t="s">
-        <v>18</v>
+      <c r="D22" s="47"/>
+      <c r="E22" s="48"/>
+      <c r="F22" s="46" t="s">
+        <v>14</v>
       </c>
-      <c r="G22" s="72"/>
-      <c r="H22" s="73"/>
-      <c r="I22" s="71" t="s">
-        <v>19</v>
+      <c r="G22" s="47"/>
+      <c r="H22" s="48"/>
+      <c r="I22" s="46" t="s">
+        <v>15</v>
       </c>
-      <c r="J22" s="73"/>
+      <c r="J22" s="48"/>
       <c r="K22" s="7"/>
       <c r="L22" s="4"/>
       <c r="M22" s="4"/>
@@ -21091,16 +21059,16 @@
       <c r="B23" s="14">
         <v>1</v>
       </c>
-      <c r="C23" s="54" t="s">
-        <v>20</v>
+      <c r="C23" s="49" t="s">
+        <v>16</v>
       </c>
-      <c r="D23" s="55"/>
-      <c r="E23" s="56"/>
-      <c r="F23" s="57"/>
-      <c r="G23" s="58"/>
-      <c r="H23" s="59"/>
-      <c r="I23" s="60"/>
-      <c r="J23" s="61"/>
+      <c r="D23" s="50"/>
+      <c r="E23" s="51"/>
+      <c r="F23" s="52"/>
+      <c r="G23" s="53"/>
+      <c r="H23" s="54"/>
+      <c r="I23" s="55"/>
+      <c r="J23" s="56"/>
       <c r="K23" s="7"/>
       <c r="L23" s="4"/>
       <c r="M23" s="4"/>
@@ -21113,20 +21081,20 @@
       <c r="B24" s="15">
         <v>2</v>
       </c>
-      <c r="C24" s="30" t="s">
-        <v>21</v>
+      <c r="C24" s="57" t="s">
+        <v>17</v>
       </c>
-      <c r="D24" s="31"/>
-      <c r="E24" s="32"/>
-      <c r="F24" s="62" t="s">
-        <v>38</v>
+      <c r="D24" s="58"/>
+      <c r="E24" s="59"/>
+      <c r="F24" s="60" t="s">
+        <v>34</v>
       </c>
-      <c r="G24" s="63"/>
-      <c r="H24" s="64"/>
-      <c r="I24" s="65" t="s">
-        <v>38</v>
+      <c r="G24" s="61"/>
+      <c r="H24" s="62"/>
+      <c r="I24" s="63" t="s">
+        <v>34</v>
       </c>
-      <c r="J24" s="66"/>
+      <c r="J24" s="64"/>
       <c r="K24" s="7"/>
       <c r="L24" s="4"/>
       <c r="M24" s="4"/>
@@ -21139,20 +21107,20 @@
       <c r="B25" s="15">
         <v>3</v>
       </c>
-      <c r="C25" s="30" t="s">
-        <v>22</v>
+      <c r="C25" s="57" t="s">
+        <v>18</v>
       </c>
-      <c r="D25" s="31"/>
-      <c r="E25" s="32"/>
-      <c r="F25" s="50" t="s">
-        <v>23</v>
+      <c r="D25" s="58"/>
+      <c r="E25" s="59"/>
+      <c r="F25" s="70" t="s">
+        <v>19</v>
       </c>
-      <c r="G25" s="51"/>
-      <c r="H25" s="52"/>
-      <c r="I25" s="53" t="s">
-        <v>24</v>
+      <c r="G25" s="71"/>
+      <c r="H25" s="72"/>
+      <c r="I25" s="73" t="s">
+        <v>20</v>
       </c>
-      <c r="J25" s="35"/>
+      <c r="J25" s="74"/>
       <c r="K25" s="7"/>
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
@@ -21165,18 +21133,18 @@
       <c r="B26" s="15">
         <v>4</v>
       </c>
-      <c r="C26" s="30" t="s">
-        <v>25</v>
+      <c r="C26" s="57" t="s">
+        <v>21</v>
       </c>
-      <c r="D26" s="31"/>
+      <c r="D26" s="58"/>
       <c r="E26" s="16" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
-      <c r="F26" s="45"/>
-      <c r="G26" s="46"/>
-      <c r="H26" s="47"/>
-      <c r="I26" s="48"/>
-      <c r="J26" s="49"/>
+      <c r="F26" s="65"/>
+      <c r="G26" s="66"/>
+      <c r="H26" s="67"/>
+      <c r="I26" s="68"/>
+      <c r="J26" s="69"/>
       <c r="K26" s="7"/>
       <c r="L26" s="4"/>
       <c r="M26" s="4"/>
@@ -21189,16 +21157,16 @@
       <c r="B27" s="15">
         <v>5</v>
       </c>
-      <c r="C27" s="30"/>
-      <c r="D27" s="31"/>
+      <c r="C27" s="57"/>
+      <c r="D27" s="58"/>
       <c r="E27" s="16" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
-      <c r="F27" s="45"/>
-      <c r="G27" s="46"/>
-      <c r="H27" s="47"/>
-      <c r="I27" s="48"/>
-      <c r="J27" s="49"/>
+      <c r="F27" s="65"/>
+      <c r="G27" s="66"/>
+      <c r="H27" s="67"/>
+      <c r="I27" s="68"/>
+      <c r="J27" s="69"/>
       <c r="K27" s="7"/>
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
@@ -21211,18 +21179,18 @@
       <c r="B28" s="15">
         <v>6</v>
       </c>
-      <c r="C28" s="30" t="s">
-        <v>28</v>
+      <c r="C28" s="57" t="s">
+        <v>24</v>
       </c>
-      <c r="D28" s="31"/>
+      <c r="D28" s="58"/>
       <c r="E28" s="16" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
-      <c r="F28" s="45"/>
-      <c r="G28" s="46"/>
-      <c r="H28" s="47"/>
-      <c r="I28" s="48"/>
-      <c r="J28" s="49"/>
+      <c r="F28" s="65"/>
+      <c r="G28" s="66"/>
+      <c r="H28" s="67"/>
+      <c r="I28" s="68"/>
+      <c r="J28" s="69"/>
       <c r="K28" s="7"/>
       <c r="L28" s="4"/>
       <c r="M28" s="4"/>
@@ -21235,16 +21203,16 @@
       <c r="B29" s="15">
         <v>7</v>
       </c>
-      <c r="C29" s="30"/>
-      <c r="D29" s="31"/>
+      <c r="C29" s="57"/>
+      <c r="D29" s="58"/>
       <c r="E29" s="16" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
-      <c r="F29" s="45"/>
-      <c r="G29" s="46"/>
-      <c r="H29" s="47"/>
-      <c r="I29" s="48"/>
-      <c r="J29" s="49"/>
+      <c r="F29" s="65"/>
+      <c r="G29" s="66"/>
+      <c r="H29" s="67"/>
+      <c r="I29" s="68"/>
+      <c r="J29" s="69"/>
       <c r="K29" s="7"/>
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
@@ -21257,16 +21225,16 @@
       <c r="B30" s="15">
         <v>8</v>
       </c>
-      <c r="C30" s="30" t="s">
-        <v>29</v>
+      <c r="C30" s="57" t="s">
+        <v>25</v>
       </c>
-      <c r="D30" s="31"/>
-      <c r="E30" s="32"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="46"/>
-      <c r="H30" s="47"/>
-      <c r="I30" s="48"/>
-      <c r="J30" s="49"/>
+      <c r="D30" s="58"/>
+      <c r="E30" s="59"/>
+      <c r="F30" s="65"/>
+      <c r="G30" s="66"/>
+      <c r="H30" s="67"/>
+      <c r="I30" s="68"/>
+      <c r="J30" s="69"/>
       <c r="K30" s="7"/>
       <c r="L30" s="4"/>
       <c r="M30" s="4"/>
@@ -21279,16 +21247,16 @@
       <c r="B31" s="15">
         <v>9</v>
       </c>
-      <c r="C31" s="30" t="s">
-        <v>30</v>
+      <c r="C31" s="57" t="s">
+        <v>26</v>
       </c>
-      <c r="D31" s="31"/>
-      <c r="E31" s="32"/>
-      <c r="F31" s="33"/>
-      <c r="G31" s="34"/>
-      <c r="H31" s="35"/>
-      <c r="I31" s="36"/>
-      <c r="J31" s="35"/>
+      <c r="D31" s="58"/>
+      <c r="E31" s="59"/>
+      <c r="F31" s="75"/>
+      <c r="G31" s="76"/>
+      <c r="H31" s="74"/>
+      <c r="I31" s="77"/>
+      <c r="J31" s="74"/>
       <c r="K31" s="7"/>
       <c r="L31" s="4"/>
       <c r="M31" s="4"/>
@@ -21301,16 +21269,16 @@
       <c r="B32" s="17">
         <v>10</v>
       </c>
-      <c r="C32" s="37" t="s">
-        <v>31</v>
+      <c r="C32" s="78" t="s">
+        <v>27</v>
       </c>
-      <c r="D32" s="38"/>
-      <c r="E32" s="39"/>
-      <c r="F32" s="40"/>
-      <c r="G32" s="41"/>
-      <c r="H32" s="42"/>
-      <c r="I32" s="43"/>
-      <c r="J32" s="44"/>
+      <c r="D32" s="79"/>
+      <c r="E32" s="80"/>
+      <c r="F32" s="81"/>
+      <c r="G32" s="82"/>
+      <c r="H32" s="83"/>
+      <c r="I32" s="84"/>
+      <c r="J32" s="85"/>
       <c r="K32" s="7"/>
       <c r="L32" s="4"/>
       <c r="M32" s="4"/>
@@ -21320,20 +21288,20 @@
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A33" s="5"/>
-      <c r="B33" s="24" t="s">
-        <v>32</v>
+      <c r="B33" s="26" t="s">
+        <v>28</v>
       </c>
-      <c r="C33" s="24"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="25" t="s">
-        <v>33</v>
+      <c r="C33" s="26"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="86" t="s">
+        <v>29</v>
       </c>
-      <c r="F33" s="25"/>
-      <c r="G33" s="25"/>
-      <c r="H33" s="25"/>
-      <c r="I33" s="25"/>
-      <c r="J33" s="25"/>
-      <c r="K33" s="26"/>
+      <c r="F33" s="86"/>
+      <c r="G33" s="86"/>
+      <c r="H33" s="86"/>
+      <c r="I33" s="86"/>
+      <c r="J33" s="86"/>
+      <c r="K33" s="87"/>
       <c r="L33" s="4"/>
       <c r="M33" s="4"/>
       <c r="N33" s="4"/>
@@ -21345,15 +21313,15 @@
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
-      <c r="E34" s="27" t="s">
-        <v>10</v>
+      <c r="E34" s="88" t="s">
+        <v>6</v>
       </c>
-      <c r="F34" s="27"/>
-      <c r="G34" s="27"/>
-      <c r="H34" s="27"/>
-      <c r="I34" s="27"/>
-      <c r="J34" s="27"/>
-      <c r="K34" s="28"/>
+      <c r="F34" s="88"/>
+      <c r="G34" s="88"/>
+      <c r="H34" s="88"/>
+      <c r="I34" s="88"/>
+      <c r="J34" s="88"/>
+      <c r="K34" s="89"/>
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
       <c r="N34" s="4"/>
@@ -21362,16 +21330,16 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A35" s="5"/>
-      <c r="B35" s="23" t="s">
-        <v>34</v>
+      <c r="B35" s="39" t="s">
+        <v>30</v>
       </c>
-      <c r="C35" s="23"/>
-      <c r="D35" s="23"/>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
-      <c r="G35" s="23"/>
-      <c r="H35" s="23"/>
-      <c r="I35" s="23"/>
+      <c r="C35" s="39"/>
+      <c r="D35" s="39"/>
+      <c r="E35" s="39"/>
+      <c r="F35" s="39"/>
+      <c r="G35" s="39"/>
+      <c r="H35" s="39"/>
+      <c r="I35" s="39"/>
       <c r="J35" s="6"/>
       <c r="K35" s="7"/>
       <c r="L35" s="4"/>
@@ -21382,17 +21350,17 @@
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A36" s="5"/>
-      <c r="B36" s="29" t="str">
+      <c r="B36" s="90" t="str">
         <f>CONCATENATE("ООО Нова Ролл Пак №",E14," ",E20)</f>
         <v>ООО Нова Ролл Пак №1349 18.08.2022 г.</v>
       </c>
-      <c r="C36" s="29"/>
-      <c r="D36" s="29"/>
-      <c r="E36" s="29"/>
-      <c r="F36" s="29"/>
-      <c r="G36" s="29"/>
-      <c r="H36" s="29"/>
-      <c r="I36" s="29"/>
+      <c r="C36" s="90"/>
+      <c r="D36" s="90"/>
+      <c r="E36" s="90"/>
+      <c r="F36" s="90"/>
+      <c r="G36" s="90"/>
+      <c r="H36" s="90"/>
+      <c r="I36" s="90"/>
       <c r="J36" s="6"/>
       <c r="K36" s="7"/>
       <c r="L36" s="4"/>
@@ -21403,9 +21371,9 @@
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A37" s="5"/>
-      <c r="B37" s="23"/>
-      <c r="C37" s="23"/>
-      <c r="D37" s="23"/>
+      <c r="B37" s="39"/>
+      <c r="C37" s="39"/>
+      <c r="D37" s="39"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
@@ -21421,11 +21389,11 @@
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A38" s="5"/>
-      <c r="B38" s="23" t="s">
-        <v>35</v>
+      <c r="B38" s="39" t="s">
+        <v>31</v>
       </c>
-      <c r="C38" s="23"/>
-      <c r="D38" s="23"/>
+      <c r="C38" s="39"/>
+      <c r="D38" s="39"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
@@ -21441,19 +21409,19 @@
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A39" s="5"/>
-      <c r="B39" s="23" t="s">
-        <v>36</v>
+      <c r="B39" s="39" t="s">
+        <v>32</v>
       </c>
-      <c r="C39" s="23"/>
-      <c r="D39" s="23"/>
+      <c r="C39" s="39"/>
+      <c r="D39" s="39"/>
       <c r="E39" s="18"/>
       <c r="F39" s="18"/>
       <c r="G39" s="18"/>
       <c r="H39" s="18"/>
-      <c r="I39" s="23" t="s">
-        <v>37</v>
+      <c r="I39" s="39" t="s">
+        <v>33</v>
       </c>
-      <c r="J39" s="23"/>
+      <c r="J39" s="39"/>
       <c r="K39" s="7"/>
       <c r="L39" s="4"/>
       <c r="M39" s="4"/>
@@ -21484,39 +21452,21 @@
     <protectedRange sqref="G8 C11:J11 H14:I14 M9:P11 F23:H23 I23:J24 F26:J30 I32:J32 B36:I36" name="Формулы"/>
   </protectedRanges>
   <mergeCells count="64">
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="E10:J10"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
-    <mergeCell ref="A6:K6"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="C12:J12"/>
-    <mergeCell ref="B13:J13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="B15:I15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="B17:I17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E18:I18"/>
-    <mergeCell ref="B19:I19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="E20:I20"/>
-    <mergeCell ref="B21:I21"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="E33:K33"/>
+    <mergeCell ref="E34:K34"/>
+    <mergeCell ref="B35:I35"/>
+    <mergeCell ref="B36:I36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="I32:J32"/>
     <mergeCell ref="C30:E30"/>
     <mergeCell ref="F30:H30"/>
     <mergeCell ref="I30:J30"/>
@@ -21533,21 +21483,39 @@
     <mergeCell ref="I28:J28"/>
     <mergeCell ref="F29:H29"/>
     <mergeCell ref="I29:J29"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="I39:J39"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="E33:K33"/>
-    <mergeCell ref="E34:K34"/>
-    <mergeCell ref="B35:I35"/>
-    <mergeCell ref="B36:I36"/>
-    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="E20:I20"/>
+    <mergeCell ref="B21:I21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="B15:I15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="B17:I17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="E18:I18"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="C12:J12"/>
+    <mergeCell ref="B13:J13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="E10:J10"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
+    <mergeCell ref="A6:K6"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="H8:I8"/>
   </mergeCells>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="94" orientation="portrait" r:id="rId1"/>

</xml_diff>